<commit_message>
added line notify implementation
</commit_message>
<xml_diff>
--- a/Docref/bitly+ready.xlsx
+++ b/Docref/bitly+ready.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workstuff\my-work-python-script\Docref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A185E574-F09F-4A5E-B29C-5AD8EE3A82D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7DB399-FA04-4621-9B59-606B9AFEC4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21382,7 +21382,7 @@
   <dimension ref="A1:BBY1469"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1458" workbookViewId="0">
-      <selection activeCell="D1468" sqref="D1468"/>
+      <selection activeCell="A1470" sqref="A1470"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>